<commit_message>
add a few files work on navigation
</commit_message>
<xml_diff>
--- a/_DATA185_F21_logistics.xlsx
+++ b/_DATA185_F21_logistics.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DATA185\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AF2835-33B6-4FC1-9EE3-A7CBA6D40F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED92878-762E-4DA7-A4B3-A4AF0DCB8F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="2295" windowWidth="57030" windowHeight="14460" activeTab="4" xr2:uid="{8EEF0BA9-6BF2-416B-B44A-FAFAC72DB9F4}"/>
+    <workbookView xWindow="0" yWindow="1290" windowWidth="57030" windowHeight="14460" activeTab="3" xr2:uid="{8EEF0BA9-6BF2-416B-B44A-FAFAC72DB9F4}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="4" r:id="rId1"/>
     <sheet name="module backward design" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
-    <sheet name="points" sheetId="5" r:id="rId4"/>
-    <sheet name="module backward design (2)" sheetId="8" r:id="rId5"/>
+    <sheet name="points" sheetId="5" r:id="rId3"/>
+    <sheet name="module backward design (2)" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="255">
   <si>
     <t>01</t>
   </si>
@@ -1204,6 +1203,15 @@
   <si>
     <t xml:space="preserve">How data influences our lives
 </t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>welcome</t>
   </si>
 </sst>
 </file>
@@ -1739,6 +1747,21 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="4" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1756,21 +1779,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="4" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -3055,46 +3063,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
       <c r="H1" s="55"/>
-      <c r="I1" s="73" t="s">
+      <c r="I1" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="73"/>
-      <c r="K1" s="74" t="s">
+      <c r="J1" s="78"/>
+      <c r="K1" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="69" t="s">
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="71" t="s">
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="72" t="s">
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
       <c r="Z1" s="54"/>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
+      <c r="AA1" s="74"/>
+      <c r="AB1" s="74"/>
       <c r="AC1" s="57" t="s">
         <v>31</v>
       </c>
@@ -3777,18 +3785,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B833A4-4AB1-4032-A6DC-3C08B75FF09C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762050E1-FE9A-4115-AA1E-A10365497E09}">
   <dimension ref="A1:P92"/>
   <sheetViews>
@@ -4592,331 +4588,342 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF8C835-1B70-4A57-B271-E46A75E13A7C}">
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39" defaultRowHeight="99.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="33" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="29" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" style="29" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" style="29" customWidth="1"/>
-    <col min="5" max="5" width="41.140625" style="29" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="29" customWidth="1"/>
-    <col min="7" max="7" width="77" style="29" customWidth="1"/>
-    <col min="8" max="8" width="70.7109375" style="29" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" style="78" customWidth="1"/>
-    <col min="10" max="10" width="43.140625" style="29" customWidth="1"/>
-    <col min="11" max="12" width="39" style="29"/>
-    <col min="13" max="13" width="17.5703125" style="29" customWidth="1"/>
-    <col min="14" max="14" width="29.140625" style="29" customWidth="1"/>
-    <col min="15" max="15" width="26.140625" style="29" customWidth="1"/>
-    <col min="16" max="16" width="36.42578125" style="29" customWidth="1"/>
-    <col min="17" max="17" width="39" style="29"/>
-    <col min="18" max="18" width="49.42578125" style="29" customWidth="1"/>
-    <col min="19" max="19" width="39" style="29"/>
-    <col min="20" max="20" width="31.7109375" style="29" customWidth="1"/>
-    <col min="21" max="21" width="28.5703125" style="29" customWidth="1"/>
-    <col min="22" max="22" width="26.42578125" style="29" customWidth="1"/>
-    <col min="23" max="23" width="37.28515625" style="29" customWidth="1"/>
-    <col min="24" max="24" width="29.140625" style="29" customWidth="1"/>
-    <col min="25" max="25" width="47.7109375" style="29" customWidth="1"/>
-    <col min="26" max="26" width="41.5703125" style="29" customWidth="1"/>
-    <col min="27" max="27" width="24" style="29" customWidth="1"/>
-    <col min="28" max="28" width="22.5703125" style="29" customWidth="1"/>
-    <col min="29" max="29" width="19.140625" style="29" customWidth="1"/>
-    <col min="30" max="16384" width="39" style="29"/>
+    <col min="1" max="2" width="10.28515625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="29" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" style="29" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" style="29" customWidth="1"/>
+    <col min="8" max="8" width="77" style="29" customWidth="1"/>
+    <col min="9" max="9" width="70.7109375" style="29" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" style="72" customWidth="1"/>
+    <col min="11" max="11" width="43.140625" style="29" customWidth="1"/>
+    <col min="12" max="13" width="39" style="29"/>
+    <col min="14" max="14" width="17.5703125" style="29" customWidth="1"/>
+    <col min="15" max="15" width="29.140625" style="29" customWidth="1"/>
+    <col min="16" max="16" width="26.140625" style="29" customWidth="1"/>
+    <col min="17" max="17" width="36.42578125" style="29" customWidth="1"/>
+    <col min="18" max="18" width="39" style="29"/>
+    <col min="19" max="19" width="49.42578125" style="29" customWidth="1"/>
+    <col min="20" max="20" width="39" style="29"/>
+    <col min="21" max="21" width="31.7109375" style="29" customWidth="1"/>
+    <col min="22" max="22" width="28.5703125" style="29" customWidth="1"/>
+    <col min="23" max="23" width="26.42578125" style="29" customWidth="1"/>
+    <col min="24" max="24" width="37.28515625" style="29" customWidth="1"/>
+    <col min="25" max="25" width="29.140625" style="29" customWidth="1"/>
+    <col min="26" max="26" width="47.7109375" style="29" customWidth="1"/>
+    <col min="27" max="27" width="41.5703125" style="29" customWidth="1"/>
+    <col min="28" max="28" width="24" style="29" customWidth="1"/>
+    <col min="29" max="29" width="22.5703125" style="29" customWidth="1"/>
+    <col min="30" max="30" width="19.140625" style="29" customWidth="1"/>
+    <col min="31" max="16384" width="39" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:31" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A1" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="73" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="73"/>
-      <c r="L1" s="74" t="s">
+      <c r="L1" s="78"/>
+      <c r="M1" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="69" t="s">
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="71" t="s">
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="72" t="s">
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="57" t="s">
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="74"/>
+      <c r="AD1" s="74"/>
+      <c r="AE1" s="57" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="126.75" customHeight="1">
+    <row r="2" spans="1:31" ht="126.75" customHeight="1">
       <c r="A2" s="32" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="B2" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="D2" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="E2" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="F2" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="G2" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="H2" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="I2" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="76"/>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="70"/>
+      <c r="K2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="L2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="M2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="N2" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="O2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="31" t="s">
+      <c r="P2" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="30" t="s">
+      <c r="Q2" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="Q2" s="30" t="s">
+      <c r="R2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="30" t="s">
+      <c r="S2" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="30" t="s">
+      <c r="T2" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="45" t="s">
+      <c r="U2" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="U2" s="45" t="s">
+      <c r="V2" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="V2" s="45" t="s">
+      <c r="W2" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="W2" s="45" t="s">
+      <c r="X2" s="45" t="s">
         <v>228</v>
       </c>
-      <c r="X2" s="37" t="s">
+      <c r="Y2" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="Y2" s="37" t="s">
+      <c r="Z2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" s="37" t="s">
+      <c r="AA2" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AA2" s="37" t="s">
+      <c r="AB2" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="AB2" s="38" t="s">
+      <c r="AC2" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="AC2" s="38" t="s">
+      <c r="AD2" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="AD2" s="58" t="s">
+      <c r="AE2" s="58" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="200.1" customHeight="1">
+    <row r="3" spans="1:31" ht="200.1" customHeight="1">
       <c r="A3" s="36" t="str">
         <f>schedule!A2</f>
         <v>01</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="48" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="D3" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="53"/>
+      <c r="F3" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="G3" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="H3" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="I3" s="56" t="s">
         <v>211</v>
       </c>
-      <c r="I3" s="77"/>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="71"/>
+      <c r="K3" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="L3" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="L3" s="29" t="s">
+      <c r="M3" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="29" t="s">
+      <c r="O3" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="O3" s="29" t="s">
+      <c r="P3" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="29" t="s">
+      <c r="R3" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="R3" s="29" t="s">
+      <c r="S3" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="S3" s="29" t="s">
+      <c r="T3" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="29" t="s">
+      <c r="U3" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="U3" s="48" t="s">
+      <c r="V3" s="48" t="s">
         <v>201</v>
       </c>
-      <c r="V3" s="49" t="s">
+      <c r="W3" s="49" t="s">
         <v>234</v>
       </c>
-      <c r="W3" s="48" t="s">
+      <c r="X3" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="AB3" s="52" t="s">
+      <c r="AC3" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="52" t="s">
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="52" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="185.25" customHeight="1">
-      <c r="B4" s="29" t="s">
-        <v>236</v>
-      </c>
-      <c r="C4" s="53" t="s">
+    <row r="4" spans="1:31" ht="185.25" customHeight="1">
+      <c r="A4" s="33">
+        <v>1</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="D4" s="53" t="s">
         <v>251</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="E4" s="73" t="s">
         <v>237</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="F4" s="53" t="s">
         <v>248</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="G4" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="48" t="s">
+      <c r="H4" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="I4" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="K4" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="L4" s="29" t="s">
         <v>240</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="O4" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="S4" s="29" t="s">
+      <c r="T4" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="T4" s="29" t="s">
+      <c r="U4" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="U4" s="29" t="s">
+      <c r="V4" s="29" t="s">
         <v>250</v>
       </c>
-      <c r="V4" s="29" t="s">
+      <c r="W4" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="W4" s="48" t="s">
+      <c r="X4" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="AD4" s="52" t="s">
+      <c r="AE4" s="52" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="99.95" customHeight="1">
-      <c r="U5" s="29" t="s">
+    <row r="5" spans="1:31" ht="99.95" customHeight="1">
+      <c r="V5" s="29" t="s">
         <v>247</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="Y1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
rebuild and reformat into modules
</commit_message>
<xml_diff>
--- a/_DATA185_F21_logistics.xlsx
+++ b/_DATA185_F21_logistics.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DATA185\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED92878-762E-4DA7-A4B3-A4AF0DCB8F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E545E3E2-1F46-4F98-90CC-4C4DEE51A032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1290" windowWidth="57030" windowHeight="14460" activeTab="3" xr2:uid="{8EEF0BA9-6BF2-416B-B44A-FAFAC72DB9F4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{8EEF0BA9-6BF2-416B-B44A-FAFAC72DB9F4}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="4" r:id="rId1"/>
     <sheet name="module backward design" sheetId="6" r:id="rId2"/>
     <sheet name="points" sheetId="5" r:id="rId3"/>
-    <sheet name="module backward design (2)" sheetId="8" r:id="rId4"/>
+    <sheet name="module design" sheetId="8" r:id="rId4"/>
+    <sheet name="calendar" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="313">
   <si>
     <t>01</t>
   </si>
@@ -1107,12 +1108,6 @@
 [Motivating Example](https://rstudio.cloud/project/2491796) (30 min)</t>
   </si>
   <si>
-    <t>Welcome, getting to know each other</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">* What is expected out of them during this class?  
 * How do they navigate the course materials?
@@ -1162,18 +1157,6 @@
 RSC --&gt; Canvas</t>
   </si>
   <si>
-    <t>[1] Start to form community of learners. 
-[2] Navigate the course materials, identify and understand the policies &amp; code of conduct
-[3] Give an example of the role of data in your life. [CO2e]
-[4] Create a file organizational strategy, and install software. [CO1e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Record welcome video
-* Create Discord channel
-* Setup Canvas with home page, modules, calendar, learning journal https://canvas.ou.edu/courses/163531/pages/journaling-in-canvas?module_item_id=3343436
-</t>
-  </si>
-  <si>
     <t>* No assumption of knowing how to use a computer is needed.</t>
   </si>
   <si>
@@ -1182,36 +1165,269 @@
 * Attendance on Day 2, and in Lab</t>
   </si>
   <si>
-    <t>* Group quiz 0
-* lec01</t>
-  </si>
-  <si>
-    <t>Introduction to Data Science
-Computing for the Sciences</t>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>welcome</t>
+  </si>
+  <si>
+    <t>cn00-welcome</t>
+  </si>
+  <si>
+    <t>Lab 01: Intro to Computing for Data Science</t>
+  </si>
+  <si>
+    <t>* Group quiz 0</t>
+  </si>
+  <si>
+    <t>Labor day</t>
+  </si>
+  <si>
+    <t>POSIT::CONF</t>
+  </si>
+  <si>
+    <t>Module(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome
+</t>
+  </si>
+  <si>
+    <t>Learning Materials</t>
+  </si>
+  <si>
+    <t>Computing for the Sciences</t>
+  </si>
+  <si>
+    <t>intro_ds</t>
+  </si>
+  <si>
+    <t>Data Literacy and Data Science</t>
+  </si>
+  <si>
+    <t>Discuss / Reflect</t>
   </si>
   <si>
     <t xml:space="preserve">* Answer questions about course navigation, tools, logistics
-* lec01 - What is Data Science? 
+* LJ -01: 321 bridge. What is Data Science? 
+* LJ -02: How does data influence your life?
 </t>
   </si>
   <si>
     <t>* Opening hook. PollEV: What is Data Science for Social Good?
 * Lec00 -Welcome slides. Who am I and why am I teaching this class? What is this class about? What are our goals for the term? 
-* Round robin intros. Who are you, where are you from, how does data influence your life? 
-* Schedule/Module overview. What are the goals  and deliverables for the week?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How data influences our lives
+* Round robin intros. Who are you, where are you from, why are you here? 
+* Module overview. How to navigate the course materials &amp; platforms</t>
+  </si>
+  <si>
+    <t>LJ -01: 321 bridge. What is Data Science? 
+LJ -02: How does data influence your life?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In class intros: Who are you, where are you from, why are you here? 
 </t>
   </si>
   <si>
-    <t>filename</t>
-  </si>
-  <si>
-    <t>Welcome</t>
-  </si>
-  <si>
-    <t>welcome</t>
+    <t>[1] Start to form community of learners. 
+[2] Navigate the course materials, identify and understand the policies &amp; code of conduct
+[3] Create a file organizational strategy, and install software. [CO1e]</t>
+  </si>
+  <si>
+    <t>Discord Introductions [1, 3]
+Personal Learning Journal [1]
+Quiz [2, 3]
+Lab [3]</t>
+  </si>
+  <si>
+    <t>Intro video</t>
+  </si>
+  <si>
+    <t>Do
+[associated module outcome]</t>
+  </si>
+  <si>
+    <t>[Syllabus](syllabus.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ASU Data LIteracy: What are Data](https://www.youtube.com/watch?v=yhO_t-c3yJY&amp;list=PLNrrxHpJhC8m_ifiOWl1hquDmdgvcviOt&amp;index=2) (11 min)  
+[Why should we care? Hans Rosling - How not to be ignorant about the world](https://www.ted.com/talks/hans_and_ola_rosling_how_not_to_be_ignorant_about_the_world?language=en#t-501411) (20 min)     </t>
+  </si>
+  <si>
+    <t>Big data is subjective
+ASU Misconceptions (2)</t>
+  </si>
+  <si>
+    <t>[Bit by Bit 1.1: Inkblot](https://www.bitbybitbook.com/en/1st-ed/introduction/ink-blot/)
+[Bit by Bit 1.2: Welcome to the digital Age](https://www.bitbybitbook.com/en/1st-ed/introduction/digital-age/)</t>
+  </si>
+  <si>
+    <t>Give an example of the role of data in your life. [CO2e]
+Identify different types of data [CO1a]
+Record data in a spreadsheet [CO1a]
+Identify if a data set is "Tidy" [CO1a]
+Diagram and explain the data lifecycle [CO1d]</t>
+  </si>
+  <si>
+    <t>Code of conduct</t>
+  </si>
+  <si>
+    <t>Building our learning community</t>
+  </si>
+  <si>
+    <t>Decision trees in R, 
+Chat GPT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe graphs as mathematical functions [CO2a]
+What is a mathematical function? Give an example. </t>
+  </si>
+  <si>
+    <t>Submodule</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Storytelling with data</t>
+  </si>
+  <si>
+    <t>HIPPA/IRB
+ASU Data Privacy (10)
+ASU Securing  Data (11)</t>
+  </si>
+  <si>
+    <t>Ethics</t>
+  </si>
+  <si>
+    <t>Stakeholders, ownership and influence</t>
+  </si>
+  <si>
+    <t>Intro to Mathematical models</t>
+  </si>
+  <si>
+    <t>Algorithmic fairness</t>
+  </si>
+  <si>
+    <t>New Jim Code / Race after technology / Coded Bias
+Calling bullshit - case study facial recognition
+Redlining
+credit card</t>
+  </si>
+  <si>
+    <t>Mistakes and manipulations</t>
+  </si>
+  <si>
+    <t>Getting and working with data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are stakeholders and why does it matter? 
+</t>
+  </si>
+  <si>
+    <t>Big Data and Algorithms</t>
+  </si>
+  <si>
+    <t>Big Data</t>
+  </si>
+  <si>
+    <t>Bit by Bit Ch 2</t>
+  </si>
+  <si>
+    <t>Asking Questions</t>
+  </si>
+  <si>
+    <t>Getting Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are metrics? 
+</t>
+  </si>
+  <si>
+    <t>ASU How to collect data (4)
+ASU Data in the news (5), sports (6), Elections (7), Health(8) 
+ASU Data Context (14)
+ASU Finding your own data (15)</t>
+  </si>
+  <si>
+    <t>Data Wrangling &amp; Integrity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working with data in R. Medical records, carpentries. </t>
+  </si>
+  <si>
+    <t>Organizing and summarizing data in Excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Define a stakeholder
+Identify influence of stakeholders across the Data Lifecycle [CO1d]
+Identifying stakeholder constraints and benefits, along with interests and influences in the current media environment
+Evaluate the likelihood/chance of report findings. 
+</t>
+  </si>
+  <si>
+    <t>Explain how data integrity can be maintained by using script files
+Create a reproducible data processing pipeline that explains all data collection and processing decisions in a literate and transparent manner. [CO1e]</t>
+  </si>
+  <si>
+    <t>Identify various forms of data privacy and protections
+Assess data integrity, identify potential privacy issues [CO1c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eugenics
+Ethical and responsible use of open data 1.2.2 https://aims.gitbook.io/open-data-mooc/unit-1-open-data-principles/lesson-1.2-ethics-in-open-data-lifecycle 
+</t>
+  </si>
+  <si>
+    <t>Bit by Bit chapter 6 is HUGE</t>
+  </si>
+  <si>
+    <t>How are analytical models related to mathematical functions? [CO2a]
+Explain why algorithms are created, and provide examples of how they are used [CO2d]
+Explain the relationship between Optimization and Analytics. [CO2b]</t>
+  </si>
+  <si>
+    <t>Mathematical Functions
+KPIs
+optimization</t>
+  </si>
+  <si>
+    <t>(ASU) What are data/data literacy (1)
+How to not be ignorant about the world [Hans Rosling]
+What does data look like
+Data Lifecycle
+Data science (back end ML) vs Data analytics (EDA) vs Stats vs CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This module provides an introduction to the field of Data Science and how it differs from traditional fields. We define what data is, explore how it's stored and used to make decisions, and some common misconceptions when dealing with data. We'll work with structured data using Excel and learn about it's properties. </t>
+  </si>
+  <si>
+    <t>Critically examine and critique data used in reports, news articles and advertisements. [CO2e]
+Interpret and draw inferences from Analytical models while taking into account the socio-political-ethical-economic implications of conclusions being made. [CO2]</t>
+  </si>
+  <si>
+    <t>Explain what it means to encode bias into an algorithm and provide an example [CO2d]
+Define algorithmic bias, feedback loop [CO2d]</t>
+  </si>
+  <si>
+    <t>Identify ways in which Data Analytics can contribute, or harm, the cultural and economic well being of diverse societies in local, national, and global scopes. [CO2c]
+Explain how the method of data collection, the involvement of stakeholders, and decisions made during data processing can have downstream impacts. [CO1]</t>
+  </si>
+  <si>
+    <t>WMD teacher value added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Import and view data in R [CO1b]
+</t>
+  </si>
+  <si>
+    <t>Reading and evaluating data dictionaries and documentation [CO1c]
+Determine the appropriateness of data for a given question [CO1c]</t>
+  </si>
+  <si>
+    <t>Observation vs Experimental (causation/correlation)</t>
   </si>
 </sst>
 </file>
@@ -1383,7 +1599,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1486,6 +1702,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -1540,7 +1762,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1554,8 +1776,11 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="4" applyAlignment="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
@@ -1747,21 +1972,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="3" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="4" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1780,8 +1990,14 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="40% - Accent3" xfId="7" builtinId="39"/>
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Accent3" xfId="6" builtinId="37"/>
@@ -1794,6 +2010,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{5DC6B65B-4C12-4AAB-8655-F7D14D0796B3}"/>
     <cellStyle name="Percent 2" xfId="4" xr:uid="{BCA2F452-C5B0-4866-BC80-4191DB955BA1}"/>
+    <cellStyle name="Style 1" xfId="13" xr:uid="{2EFC84A8-5403-4CA5-9C6D-A3655780DE88}"/>
     <cellStyle name="Total" xfId="2" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2116,7 +2333,7 @@
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C7" sqref="C7"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
@@ -3027,7 +3244,7 @@
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39" defaultRowHeight="99.95" customHeight="1"/>
@@ -3040,15 +3257,15 @@
     <col min="6" max="6" width="24.7109375" style="29" customWidth="1"/>
     <col min="7" max="7" width="77" style="29" customWidth="1"/>
     <col min="8" max="8" width="82.7109375" style="29" customWidth="1"/>
-    <col min="9" max="9" width="43.140625" style="29" customWidth="1"/>
-    <col min="10" max="11" width="39" style="29"/>
-    <col min="12" max="12" width="17.5703125" style="29" customWidth="1"/>
-    <col min="13" max="13" width="29.140625" style="29" customWidth="1"/>
-    <col min="14" max="14" width="26.140625" style="29" customWidth="1"/>
-    <col min="15" max="15" width="36.42578125" style="29" customWidth="1"/>
-    <col min="16" max="16" width="39" style="29"/>
-    <col min="17" max="17" width="49.42578125" style="29" customWidth="1"/>
-    <col min="18" max="18" width="39" style="29"/>
+    <col min="9" max="9" width="43.140625" style="29" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="0" style="29" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" style="29" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" style="29" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" style="29" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="36.42578125" style="29" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="0" style="29" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="49.42578125" style="29" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="0" style="29" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="31.7109375" style="29" customWidth="1"/>
     <col min="20" max="20" width="28.5703125" style="29" customWidth="1"/>
     <col min="21" max="21" width="30.85546875" style="29" customWidth="1"/>
@@ -3063,46 +3280,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
       <c r="H1" s="55"/>
-      <c r="I1" s="78" t="s">
+      <c r="I1" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="78"/>
-      <c r="K1" s="79" t="s">
+      <c r="J1" s="73"/>
+      <c r="K1" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="74" t="s">
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="76" t="s">
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="77" t="s">
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
+      <c r="X1" s="72"/>
+      <c r="Y1" s="72"/>
       <c r="Z1" s="54"/>
-      <c r="AA1" s="74"/>
-      <c r="AB1" s="74"/>
+      <c r="AA1" s="69"/>
+      <c r="AB1" s="69"/>
       <c r="AC1" s="57" t="s">
         <v>31</v>
       </c>
@@ -4590,104 +4807,93 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF8C835-1B70-4A57-B271-E46A75E13A7C}">
-  <dimension ref="A1:AE5"/>
+  <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="39" defaultRowHeight="99.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="39" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="10.28515625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="29" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" style="29" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" style="29" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" style="29" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" style="29" customWidth="1"/>
-    <col min="8" max="8" width="77" style="29" customWidth="1"/>
-    <col min="9" max="9" width="70.7109375" style="29" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" style="72" customWidth="1"/>
-    <col min="11" max="11" width="43.140625" style="29" customWidth="1"/>
-    <col min="12" max="13" width="39" style="29"/>
-    <col min="14" max="14" width="17.5703125" style="29" customWidth="1"/>
-    <col min="15" max="15" width="29.140625" style="29" customWidth="1"/>
-    <col min="16" max="16" width="26.140625" style="29" customWidth="1"/>
-    <col min="17" max="17" width="36.42578125" style="29" customWidth="1"/>
-    <col min="18" max="18" width="39" style="29"/>
-    <col min="19" max="19" width="49.42578125" style="29" customWidth="1"/>
-    <col min="20" max="20" width="39" style="29"/>
-    <col min="21" max="21" width="31.7109375" style="29" customWidth="1"/>
-    <col min="22" max="22" width="28.5703125" style="29" customWidth="1"/>
-    <col min="23" max="23" width="26.42578125" style="29" customWidth="1"/>
-    <col min="24" max="24" width="37.28515625" style="29" customWidth="1"/>
-    <col min="25" max="25" width="29.140625" style="29" customWidth="1"/>
-    <col min="26" max="26" width="47.7109375" style="29" customWidth="1"/>
-    <col min="27" max="27" width="41.5703125" style="29" customWidth="1"/>
-    <col min="28" max="28" width="24" style="29" customWidth="1"/>
-    <col min="29" max="29" width="22.5703125" style="29" customWidth="1"/>
-    <col min="30" max="30" width="19.140625" style="29" customWidth="1"/>
-    <col min="31" max="16384" width="39" style="29"/>
+    <col min="1" max="1" width="7.42578125" style="33" hidden="1" customWidth="1"/>
+    <col min="2" max="3" width="24.28515625" style="29" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" style="29" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" style="29" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" style="29" customWidth="1"/>
+    <col min="8" max="8" width="72.140625" style="29" customWidth="1"/>
+    <col min="9" max="9" width="56.28515625" style="29" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" style="29" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="0" style="29" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" style="29" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="29.140625" style="29" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="26.140625" style="29" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="36.42578125" style="29" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="39" style="29" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="49.42578125" style="29" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="39" style="29" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="29.140625" style="29" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="42.28515625" style="29" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="35" style="29" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="26.140625" style="29" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="24" style="29" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="22.5703125" style="29" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" style="29" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="49.5703125" style="29" hidden="1" customWidth="1"/>
+    <col min="28" max="16384" width="39" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:27" ht="19.5" thickBot="1">
+      <c r="A1" s="70"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="73"/>
+      <c r="L1" s="74" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="72" t="s">
+        <v>253</v>
+      </c>
+      <c r="U1" s="72"/>
+      <c r="V1" s="72"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="69"/>
+      <c r="Z1" s="69"/>
+      <c r="AA1" s="57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="47.25" customHeight="1">
+      <c r="A2" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="78" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="78"/>
-      <c r="M1" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="76" t="s">
-        <v>67</v>
-      </c>
-      <c r="V1" s="76"/>
-      <c r="W1" s="76"/>
-      <c r="X1" s="76"/>
-      <c r="Y1" s="77" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="74"/>
-      <c r="AD1" s="74"/>
-      <c r="AE1" s="57" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" ht="126.75" customHeight="1">
-      <c r="A2" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>252</v>
-      </c>
       <c r="C2" s="32" t="s">
-        <v>20</v>
+        <v>275</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>91</v>
@@ -4707,225 +4913,575 @@
       <c r="I2" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="70"/>
+      <c r="J2" s="28" t="s">
+        <v>14</v>
+      </c>
       <c r="K2" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="28" t="s">
         <v>15</v>
       </c>
+      <c r="L2" s="31" t="s">
+        <v>25</v>
+      </c>
       <c r="M2" s="31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" s="31" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="O2" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="31" t="s">
         <v>59</v>
       </c>
+      <c r="P2" s="30" t="s">
+        <v>72</v>
+      </c>
       <c r="Q2" s="30" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="R2" s="30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="S2" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="V2" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="W2" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="X2" s="45" t="s">
-        <v>228</v>
-      </c>
-      <c r="Y2" s="37" t="s">
+      <c r="T2" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="Z2" s="37" t="s">
+      <c r="U2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="AA2" s="37" t="s">
+      <c r="V2" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AB2" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="AC2" s="38" t="s">
+      <c r="W2" s="37" t="s">
+        <v>257</v>
+      </c>
+      <c r="X2" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="Y2" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="Z2" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA2" s="58" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="111" customHeight="1">
+      <c r="A3" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="G3" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>262</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="J3" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="N3" s="29" t="s">
         <v>242</v>
       </c>
-      <c r="AD2" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="AE2" s="58" t="s">
+      <c r="S3" s="29" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" ht="200.1" customHeight="1">
-      <c r="A3" s="36" t="str">
-        <f>schedule!A2</f>
-        <v>01</v>
-      </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="48" t="s">
-        <v>236</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="I3" s="56" t="s">
-        <v>211</v>
-      </c>
-      <c r="J3" s="71"/>
-      <c r="K3" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="L3" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="M3" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="P3" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="S3" s="29" t="s">
-        <v>71</v>
-      </c>
       <c r="T3" s="29" t="s">
-        <v>70</v>
+        <v>246</v>
       </c>
       <c r="U3" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="V3" s="48" t="s">
-        <v>201</v>
-      </c>
-      <c r="W3" s="49" t="s">
-        <v>234</v>
-      </c>
-      <c r="X3" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="AC3" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD3" s="5"/>
-      <c r="AE3" s="52" t="s">
+        <v>266</v>
+      </c>
+      <c r="V3" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="W3" s="29" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y3" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="AA3" s="52" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="185.25" customHeight="1">
-      <c r="A4" s="33">
-        <v>1</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>254</v>
+    <row r="4" spans="1:27" ht="136.5" customHeight="1">
+      <c r="A4" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>256</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>253</v>
-      </c>
-      <c r="D4" s="53" t="s">
-        <v>251</v>
-      </c>
-      <c r="E4" s="73" t="s">
-        <v>237</v>
-      </c>
-      <c r="F4" s="53" t="s">
-        <v>248</v>
-      </c>
-      <c r="G4" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="48" t="s">
-        <v>243</v>
+        <v>276</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>270</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>239</v>
-      </c>
-      <c r="K4" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="L4" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="O4" s="29" t="s">
-        <v>246</v>
-      </c>
-      <c r="T4" s="29" t="s">
-        <v>245</v>
-      </c>
-      <c r="U4" s="29" t="s">
-        <v>244</v>
-      </c>
-      <c r="V4" s="29" t="s">
-        <v>250</v>
+        <v>213</v>
+      </c>
+      <c r="U4" s="65" t="s">
+        <v>269</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>267</v>
       </c>
       <c r="W4" s="29" t="s">
-        <v>249</v>
-      </c>
-      <c r="X4" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="AE4" s="52" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" ht="99.95" customHeight="1">
-      <c r="V5" s="29" t="s">
-        <v>247</v>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="120">
+      <c r="C5" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="75">
+      <c r="B6" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="30">
+      <c r="C7" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="45">
+      <c r="C8" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="C9" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="120">
+      <c r="B10" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="45">
+      <c r="B11" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="60">
+      <c r="C12" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="90">
+      <c r="C13" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="90">
+      <c r="B14" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="120">
+      <c r="C15" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="H15" s="29" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="105">
+      <c r="C16" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>300</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="AC1:AD1"/>
+  <mergeCells count="6">
+    <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="U1:X1"/>
-    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C9BE77-9D1D-46C1-A81A-F2742E241111}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" style="29" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" style="29" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" style="29" customWidth="1"/>
+    <col min="6" max="6" width="52.28515625" style="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21">
+      <c r="A1" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="171" customHeight="1">
+      <c r="A2" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>45159</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75">
+      <c r="A3" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="7">
+        <f t="shared" ref="B3:B18" si="0">B2+7</f>
+        <v>45166</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75">
+      <c r="A4" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="7">
+        <f t="shared" si="0"/>
+        <v>45173</v>
+      </c>
+      <c r="D4" s="75" t="s">
+        <v>249</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75">
+      <c r="A5" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="7">
+        <f t="shared" si="0"/>
+        <v>45180</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="7">
+        <f t="shared" si="0"/>
+        <v>45187</v>
+      </c>
+      <c r="D6" s="75" t="s">
+        <v>250</v>
+      </c>
+      <c r="E6" s="75" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="7">
+        <f t="shared" si="0"/>
+        <v>45194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="7">
+        <f t="shared" si="0"/>
+        <v>45201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="7">
+        <f t="shared" si="0"/>
+        <v>45208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="7">
+        <f t="shared" si="0"/>
+        <v>45215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="51">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7">
+        <f t="shared" si="0"/>
+        <v>45222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="51">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7">
+        <f t="shared" si="0"/>
+        <v>45229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="51">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7">
+        <f t="shared" si="0"/>
+        <v>45236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="51">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7">
+        <f t="shared" si="0"/>
+        <v>45243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="51"/>
+      <c r="B15" s="7">
+        <f t="shared" si="0"/>
+        <v>45250</v>
+      </c>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="51">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7">
+        <f t="shared" si="0"/>
+        <v>45257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="51">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7">
+        <f t="shared" si="0"/>
+        <v>45264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="7">
+        <f t="shared" si="0"/>
+        <v>45271</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add styles, split calendar, mod lab01
</commit_message>
<xml_diff>
--- a/_DATA185_F21_logistics.xlsx
+++ b/_DATA185_F21_logistics.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DATA185\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E545E3E2-1F46-4F98-90CC-4C4DEE51A032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F68992-F157-4A48-B158-8AAC494682F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{8EEF0BA9-6BF2-416B-B44A-FAFAC72DB9F4}"/>
+    <workbookView xWindow="75" yWindow="135" windowWidth="57285" windowHeight="15615" activeTab="3" xr2:uid="{8EEF0BA9-6BF2-416B-B44A-FAFAC72DB9F4}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="4" r:id="rId1"/>
     <sheet name="module backward design" sheetId="6" r:id="rId2"/>
     <sheet name="points" sheetId="5" r:id="rId3"/>
     <sheet name="module design" sheetId="8" r:id="rId4"/>
-    <sheet name="calendar" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="319">
   <si>
     <t>01</t>
   </si>
@@ -1180,22 +1179,6 @@
     <t>Lab 01: Intro to Computing for Data Science</t>
   </si>
   <si>
-    <t>* Group quiz 0</t>
-  </si>
-  <si>
-    <t>Labor day</t>
-  </si>
-  <si>
-    <t>POSIT::CONF</t>
-  </si>
-  <si>
-    <t>Module(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welcome
-</t>
-  </si>
-  <si>
     <t>Learning Materials</t>
   </si>
   <si>
@@ -1209,22 +1192,6 @@
   </si>
   <si>
     <t>Discuss / Reflect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Answer questions about course navigation, tools, logistics
-* LJ -01: 321 bridge. What is Data Science? 
-* LJ -02: How does data influence your life?
-</t>
-  </si>
-  <si>
-    <t>* Opening hook. PollEV: What is Data Science for Social Good?
-* Lec00 -Welcome slides. Who am I and why am I teaching this class? What is this class about? What are our goals for the term? 
-* Round robin intros. Who are you, where are you from, why are you here? 
-* Module overview. How to navigate the course materials &amp; platforms</t>
-  </si>
-  <si>
-    <t>LJ -01: 321 bridge. What is Data Science? 
-LJ -02: How does data influence your life?</t>
   </si>
   <si>
     <t xml:space="preserve">In class intros: Who are you, where are you from, why are you here? 
@@ -1252,25 +1219,6 @@
     <t>[Syllabus](syllabus.html)</t>
   </si>
   <si>
-    <t xml:space="preserve">[ASU Data LIteracy: What are Data](https://www.youtube.com/watch?v=yhO_t-c3yJY&amp;list=PLNrrxHpJhC8m_ifiOWl1hquDmdgvcviOt&amp;index=2) (11 min)  
-[Why should we care? Hans Rosling - How not to be ignorant about the world](https://www.ted.com/talks/hans_and_ola_rosling_how_not_to_be_ignorant_about_the_world?language=en#t-501411) (20 min)     </t>
-  </si>
-  <si>
-    <t>Big data is subjective
-ASU Misconceptions (2)</t>
-  </si>
-  <si>
-    <t>[Bit by Bit 1.1: Inkblot](https://www.bitbybitbook.com/en/1st-ed/introduction/ink-blot/)
-[Bit by Bit 1.2: Welcome to the digital Age](https://www.bitbybitbook.com/en/1st-ed/introduction/digital-age/)</t>
-  </si>
-  <si>
-    <t>Give an example of the role of data in your life. [CO2e]
-Identify different types of data [CO1a]
-Record data in a spreadsheet [CO1a]
-Identify if a data set is "Tidy" [CO1a]
-Diagram and explain the data lifecycle [CO1d]</t>
-  </si>
-  <si>
     <t>Code of conduct</t>
   </si>
   <si>
@@ -1286,9 +1234,6 @@
   </si>
   <si>
     <t>Submodule</t>
-  </si>
-  <si>
-    <t>Introduction</t>
   </si>
   <si>
     <t>Storytelling with data</t>
@@ -1353,12 +1298,6 @@
   </si>
   <si>
     <t>Data Wrangling &amp; Integrity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Working with data in R. Medical records, carpentries. </t>
-  </si>
-  <si>
-    <t>Organizing and summarizing data in Excel</t>
   </si>
   <si>
     <t xml:space="preserve">Define a stakeholder
@@ -1394,40 +1333,147 @@
 optimization</t>
   </si>
   <si>
+    <t>Critically examine and critique data used in reports, news articles and advertisements. [CO2e]
+Interpret and draw inferences from Analytical models while taking into account the socio-political-ethical-economic implications of conclusions being made. [CO2]</t>
+  </si>
+  <si>
+    <t>Explain what it means to encode bias into an algorithm and provide an example [CO2d]
+Define algorithmic bias, feedback loop [CO2d]</t>
+  </si>
+  <si>
+    <t>Identify ways in which Data Analytics can contribute, or harm, the cultural and economic well being of diverse societies in local, national, and global scopes. [CO2c]
+Explain how the method of data collection, the involvement of stakeholders, and decisions made during data processing can have downstream impacts. [CO1]</t>
+  </si>
+  <si>
+    <t>WMD teacher value added</t>
+  </si>
+  <si>
+    <t>Data Literacy</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give an example of the role of data in your life. [CO2e]
+Identify different types of data [CO1a]
+Record data in a spreadsheet [CO1a]
+</t>
+  </si>
+  <si>
+    <t>Different types of black boxes (regression, classification, supervised, unsupervised, numerical vs graphical vs LLN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Lifecycle
+Data science (back end ML) vs Data analytics (EDA) vs Stats vs CS
+Estimation, Inference and Prediction/Forecasing
+</t>
+  </si>
+  <si>
+    <t>Diagram and explain the data lifecycle [CO1d]
+Provide examples of different types of DS models [CO2d]</t>
+  </si>
+  <si>
+    <t>Data basics (ims 1.2)
+Organizing and summarizing data in Excel</t>
+  </si>
+  <si>
     <t>(ASU) What are data/data literacy (1)
 How to not be ignorant about the world [Hans Rosling]
-What does data look like
-Data Lifecycle
-Data science (back end ML) vs Data analytics (EDA) vs Stats vs CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This module provides an introduction to the field of Data Science and how it differs from traditional fields. We define what data is, explore how it's stored and used to make decisions, and some common misconceptions when dealing with data. We'll work with structured data using Excel and learn about it's properties. </t>
-  </si>
-  <si>
-    <t>Critically examine and critique data used in reports, news articles and advertisements. [CO2e]
-Interpret and draw inferences from Analytical models while taking into account the socio-political-ethical-economic implications of conclusions being made. [CO2]</t>
-  </si>
-  <si>
-    <t>Explain what it means to encode bias into an algorithm and provide an example [CO2d]
-Define algorithmic bias, feedback loop [CO2d]</t>
-  </si>
-  <si>
-    <t>Identify ways in which Data Analytics can contribute, or harm, the cultural and economic well being of diverse societies in local, national, and global scopes. [CO2c]
-Explain how the method of data collection, the involvement of stakeholders, and decisions made during data processing can have downstream impacts. [CO1]</t>
-  </si>
-  <si>
-    <t>WMD teacher value added</t>
+Motivating examples (introductions)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data science is an interdisciplinary field focused on extracting knowledge from typically large data sets and applying the knowledge and insights from that data to solve problems in a wide range of application domains [cite](https://en.wikipedia.org/wiki/Data_science). This lesson provides an introduction to the field of Data Science and how it differs from traditional fields, and provides examples of some of the common types of Data Science models that are used to make decisions. </t>
+  </si>
+  <si>
+    <t>Data Literacy is the ability to read, understand, create and communicate data as information [cite](https://en.wikipedia.org/wiki/Data_literacy). This lesson covers some motivating examples of how data have been used to make decisions, necessary terminology for talking about data, and some hands on experience with organizing and summarizing data in a spreadsheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Causality and Experiments
+</t>
+  </si>
+  <si>
+    <t>Observation vs Experimental (causation/correlation)
+Observational data and Big data</t>
+  </si>
+  <si>
+    <t>Working with data in R. R4DS data viz</t>
+  </si>
+  <si>
+    <t>Literate reporting with Quarto
+select, filter, mutate</t>
   </si>
   <si>
     <t xml:space="preserve">Import and view data in R [CO1b]
+Reading and evaluating data dictionaries and documentation [CO1c]
+Determine the appropriateness of data for a given question [CO1c]
 </t>
   </si>
   <si>
-    <t>Reading and evaluating data dictionaries and documentation [CO1c]
-Determine the appropriateness of data for a given question [CO1c]</t>
-  </si>
-  <si>
-    <t>Observation vs Experimental (causation/correlation)</t>
+    <t>LJ -02: How does data influence your life?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">act01 - toolkit
+LJ -01: 321 bridge. What is Data Science? </t>
+  </si>
+  <si>
+    <t>ASU Misconceptions (2)
+Calling bullshit - misleading axes, proportional ink</t>
+  </si>
+  <si>
+    <t>[Data8 Ch 2. Causality and Experiments](https://inferentialthinking.com/chapters/02/causality-and-experiments.html)
+[Why the term "Data Science" is confusing](https://www.quora.com/What-is-data-science/answer/Michael-Hochster)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cn01-intro-ds (data literacy, data lifecycle, data science overview)
+cn02-data-basics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  (build from https://github.com/OpenIntroStat/ims/blob/main/01-data-hello.Rmd)</t>
+    </r>
+  </si>
+  <si>
+    <t>Lab 02: Intro to Excel</t>
+  </si>
+  <si>
+    <t>[BBB 1.1: Inkblot](https://www.bitbybitbook.com/en/1st-ed/introduction/ink-blot/)</t>
+  </si>
+  <si>
+    <t>[BBB 1.2: Welcome to the digital Age](https://www.bitbybitbook.com/en/1st-ed/introduction/digital-age/)
+[R4DS Intro](https://r4ds.hadley.nz/intro.html)
+[Data8 1](What is Data Science (https://inferentialthinking.com/chapters/01/what-is-data-science.html)
+[Data8 1.1](Intro https://inferentialthinking.com/chapters/01/1/intro.html)
+[Data8 1.1.2](Statistical Techniques https://inferentialthinking.com/chapters/01/1/2/statistical-techniques.html)
+[Data8 1.2](Why Data Science https://inferentialthinking.com/chapters/01/2/why-data-science.html)
+[IMS 1.2](Data Basics https://openintro-ims.netlify.app/data-hello.html#data-basics)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* [Share out] Google "day in the life of a data scientist" or "data analyst"  or "how to become a data scientist" and and find someone that resonates with you. Share the  link in discord, and briefly describe what you learned from them. (https://www.youtube.com/watch?v=5O9abIxIqNA, https://www.youtube.com/watch?v=Z79AqDouS-Y) 
+* [connect] Watch and comment on at least one other persons post. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ASU: What are Data](https://www.youtube.com/watch?v=yhO_t-c3yJY&amp;list=PLNrrxHpJhC8m_ifiOWl1hquDmdgvcviOt&amp;index=2) (11 min)  
+[How not to be ignorant about the world](https://www.ted.com/talks/hans_and_ola_rosling_how_not_to_be_ignorant_about_the_world) (20 min)     
+</t>
+  </si>
+  <si>
+    <t>[ASU: Misconceptions in Data Analysis](https://www.youtube.com/watch?v=nd_oOOXeN3A&amp;list=PLNrrxHpJhC8m_ifiOWl1hquDmdgvcviOt&amp;index=3) (10 min)</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1645,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1702,12 +1748,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -1990,10 +2030,10 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2330,10 +2370,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D366DCB5-0C09-4243-87DB-31A18924021A}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C7" sqref="C7"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
@@ -3244,7 +3284,7 @@
       <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4:H8"/>
+      <selection pane="bottomRight" activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39" defaultRowHeight="99.95" customHeight="1"/>
@@ -4807,42 +4847,44 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF8C835-1B70-4A57-B271-E46A75E13A7C}">
-  <dimension ref="A1:AA16"/>
+  <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.42578125" style="33" hidden="1" customWidth="1"/>
-    <col min="2" max="3" width="24.28515625" style="29" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="29" customWidth="1"/>
     <col min="4" max="4" width="32.5703125" style="29" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" style="29" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" style="29" customWidth="1"/>
     <col min="7" max="7" width="43.7109375" style="29" customWidth="1"/>
-    <col min="8" max="8" width="72.140625" style="29" customWidth="1"/>
+    <col min="8" max="8" width="46.7109375" style="29" customWidth="1"/>
     <col min="9" max="9" width="56.28515625" style="29" customWidth="1"/>
     <col min="10" max="10" width="43.140625" style="29" hidden="1" customWidth="1"/>
-    <col min="11" max="12" width="0" style="29" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" style="29" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="29.140625" style="29" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="26.140625" style="29" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="39" style="29" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="39" style="29" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" style="29" customWidth="1"/>
+    <col min="14" max="14" width="29.140625" style="29" customWidth="1"/>
+    <col min="15" max="15" width="26.140625" style="29" customWidth="1"/>
     <col min="16" max="16" width="36.42578125" style="29" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="39" style="29" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="49.42578125" style="29" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="39" style="29" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="29.140625" style="29" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="42.28515625" style="29" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="35" style="29" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="26.140625" style="29" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="24" style="29" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="22.5703125" style="29" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="19.140625" style="29" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="49.5703125" style="29" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="29.140625" style="29" customWidth="1"/>
+    <col min="21" max="21" width="42.28515625" style="29" customWidth="1"/>
+    <col min="22" max="22" width="35" style="29" customWidth="1"/>
+    <col min="23" max="23" width="26.140625" style="29" customWidth="1"/>
+    <col min="24" max="24" width="24" style="29" customWidth="1"/>
+    <col min="25" max="25" width="22.5703125" style="29" customWidth="1"/>
+    <col min="26" max="26" width="19.140625" style="29" customWidth="1"/>
+    <col min="27" max="27" width="49.5703125" style="29" customWidth="1"/>
     <col min="28" max="16384" width="39" style="29"/>
   </cols>
   <sheetData>
@@ -4873,7 +4915,7 @@
       <c r="R1" s="69"/>
       <c r="S1" s="69"/>
       <c r="T1" s="72" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="U1" s="72"/>
       <c r="V1" s="72"/>
@@ -4893,7 +4935,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>91</v>
@@ -4953,10 +4995,10 @@
         <v>64</v>
       </c>
       <c r="W2" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="X2" s="37" t="s">
         <v>257</v>
-      </c>
-      <c r="X2" s="37" t="s">
-        <v>265</v>
       </c>
       <c r="Y2" s="38" t="s">
         <v>240</v>
@@ -4976,19 +5018,19 @@
         <v>244</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="G3" s="29" t="s">
         <v>85</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>237</v>
@@ -5000,7 +5042,7 @@
         <v>238</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="N3" s="29" t="s">
         <v>242</v>
@@ -5008,17 +5050,20 @@
       <c r="S3" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="T3" s="29" t="s">
+      <c r="T3" s="75" t="s">
         <v>246</v>
       </c>
       <c r="U3" s="29" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="V3" s="29" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="W3" s="29" t="s">
-        <v>261</v>
+        <v>253</v>
+      </c>
+      <c r="X3" s="29" t="s">
+        <v>309</v>
       </c>
       <c r="Y3" s="29" t="s">
         <v>247</v>
@@ -5029,99 +5074,117 @@
     </row>
     <row r="4" spans="1:27" ht="136.5" customHeight="1">
       <c r="A4" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>276</v>
+        <v>293</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>304</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>268</v>
+        <v>300</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>126</v>
+        <v>299</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>270</v>
+        <v>295</v>
       </c>
       <c r="I4" s="29" t="s">
         <v>213</v>
       </c>
+      <c r="T4" s="76" t="s">
+        <v>312</v>
+      </c>
       <c r="U4" s="65" t="s">
-        <v>269</v>
+        <v>315</v>
       </c>
       <c r="V4" s="3" t="s">
-        <v>267</v>
+        <v>317</v>
       </c>
       <c r="W4" s="29" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="120">
+        <v>314</v>
+      </c>
+      <c r="X4" s="29" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y4" s="29" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="136.5" customHeight="1">
       <c r="C5" s="29" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>134</v>
+        <v>297</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>135</v>
+        <v>303</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>296</v>
       </c>
+      <c r="G5" s="29" t="s">
+        <v>301</v>
+      </c>
       <c r="H5" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="U5" s="65" t="s">
+        <v>311</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="120">
+      <c r="B6" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="H6" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I6" s="29" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" ht="75">
-      <c r="B6" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>291</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>312</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>295</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="30">
+      <c r="V6" s="29" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="90">
       <c r="C7" s="29" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="45">
       <c r="C8" s="29" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>139</v>
@@ -5130,10 +5193,10 @@
         <v>140</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>138</v>
+        <v>306</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="I8" s="29" t="s">
         <v>141</v>
@@ -5141,18 +5204,18 @@
     </row>
     <row r="9" spans="1:27">
       <c r="C9" s="29" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="120">
       <c r="B10" s="29" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="E10" s="29" t="s">
         <v>143</v>
@@ -5161,91 +5224,102 @@
         <v>136</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="I10" s="29" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="45">
-      <c r="B11" s="29" t="s">
+    <row r="11" spans="1:27" ht="30">
+      <c r="C11" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="45">
+      <c r="B12" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="60">
+      <c r="C13" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>261</v>
+      </c>
+      <c r="H13" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>281</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>303</v>
-      </c>
-      <c r="H11" s="29" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="60">
-      <c r="C12" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="29" t="s">
-        <v>273</v>
-      </c>
-      <c r="H12" s="29" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="90">
-      <c r="C13" s="29" t="s">
-        <v>282</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>283</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>307</v>
-      </c>
     </row>
     <row r="14" spans="1:27" ht="90">
-      <c r="B14" s="29" t="s">
-        <v>279</v>
-      </c>
       <c r="C14" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="90">
+      <c r="B15" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="H15" s="29" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="120">
+      <c r="C16" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" ht="105">
+      <c r="C17" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="H17" s="29" t="s">
         <v>284</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>301</v>
-      </c>
-      <c r="H14" s="29" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" ht="120">
-      <c r="C15" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="H15" s="29" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" ht="105">
-      <c r="C16" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>278</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>300</v>
-      </c>
-      <c r="H16" s="29" t="s">
-        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -5260,228 +5334,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C9BE77-9D1D-46C1-A81A-F2742E241111}">
-  <dimension ref="A1:F18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.5703125" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" style="29" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" style="29" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" style="29" customWidth="1"/>
-    <col min="6" max="6" width="52.28515625" style="29" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="21">
-      <c r="A1" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>251</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="171" customHeight="1">
-      <c r="A2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7">
-        <v>45159</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>252</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>259</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>258</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75">
-      <c r="A3" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="7">
-        <f t="shared" ref="B3:B18" si="0">B2+7</f>
-        <v>45166</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>248</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75">
-      <c r="A4" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="7">
-        <f t="shared" si="0"/>
-        <v>45173</v>
-      </c>
-      <c r="D4" s="75" t="s">
-        <v>249</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75">
-      <c r="A5" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="7">
-        <f t="shared" si="0"/>
-        <v>45180</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="7">
-        <f t="shared" si="0"/>
-        <v>45187</v>
-      </c>
-      <c r="D6" s="75" t="s">
-        <v>250</v>
-      </c>
-      <c r="E6" s="75" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="7">
-        <f t="shared" si="0"/>
-        <v>45194</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="7">
-        <f t="shared" si="0"/>
-        <v>45201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="7">
-        <f t="shared" si="0"/>
-        <v>45208</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="7">
-        <f t="shared" si="0"/>
-        <v>45215</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="51">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7">
-        <f t="shared" si="0"/>
-        <v>45222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="51">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7">
-        <f t="shared" si="0"/>
-        <v>45229</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="51">
-        <v>12</v>
-      </c>
-      <c r="B13" s="7">
-        <f t="shared" si="0"/>
-        <v>45236</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="51">
-        <v>13</v>
-      </c>
-      <c r="B14" s="7">
-        <f t="shared" si="0"/>
-        <v>45243</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="51"/>
-      <c r="B15" s="7">
-        <f t="shared" si="0"/>
-        <v>45250</v>
-      </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="51">
-        <v>14</v>
-      </c>
-      <c r="B16" s="7">
-        <f t="shared" si="0"/>
-        <v>45257</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="51">
-        <v>15</v>
-      </c>
-      <c r="B17" s="7">
-        <f t="shared" si="0"/>
-        <v>45264</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="7">
-        <f t="shared" si="0"/>
-        <v>45271</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>